<commit_message>
Finished first draft of project plan
</commit_message>
<xml_diff>
--- a/HW 1/Project Plan.xlsx
+++ b/HW 1/Project Plan.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marakovitsm/Github/capping/HW 1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="180" yWindow="0" windowWidth="25260" windowHeight="12200" activeTab="1"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="25600" windowHeight="14400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project Timeline" sheetId="1" r:id="rId1"/>
@@ -17,7 +22,7 @@
     <definedName name="ProjectEnd">'Project Timeline'!$L$21</definedName>
     <definedName name="ProjectStart">'Project Timeline'!$L$19</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="153">
   <si>
     <t>Project Start</t>
   </si>
@@ -1302,8 +1307,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.11206097854822998"/>
-                      <c:h val="4.7831682330031315E-2"/>
+                      <c:w val="0.11206097854823"/>
+                      <c:h val="0.0478316823300313"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -1328,8 +1333,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.11206097854822998"/>
-                      <c:h val="4.7831682330031315E-2"/>
+                      <c:w val="0.11206097854823"/>
+                      <c:h val="0.0478316823300313"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -1354,8 +1359,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.11206097854822998"/>
-                      <c:h val="4.7831682330031315E-2"/>
+                      <c:w val="0.11206097854823"/>
+                      <c:h val="0.0478316823300313"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -1380,8 +1385,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.11206097854822998"/>
-                      <c:h val="4.7831682330031315E-2"/>
+                      <c:w val="0.11206097854823"/>
+                      <c:h val="0.0478316823300313"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -1406,8 +1411,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.11206097854822998"/>
-                      <c:h val="4.7831682330031315E-2"/>
+                      <c:w val="0.11206097854823"/>
+                      <c:h val="0.0478316823300313"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -1432,8 +1437,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.11206097854822998"/>
-                      <c:h val="4.7831682330031315E-2"/>
+                      <c:w val="0.11206097854823"/>
+                      <c:h val="0.0478316823300313"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -1458,8 +1463,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.11206097854822998"/>
-                      <c:h val="4.7831682330031315E-2"/>
+                      <c:w val="0.11206097854823"/>
+                      <c:h val="0.0478316823300313"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -1484,8 +1489,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.11206097854822998"/>
-                      <c:h val="4.7831682330031315E-2"/>
+                      <c:w val="0.11206097854823"/>
+                      <c:h val="0.0478316823300313"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -1510,8 +1515,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.11206097854822998"/>
-                      <c:h val="4.7831682330031315E-2"/>
+                      <c:w val="0.11206097854823"/>
+                      <c:h val="0.0478316823300313"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -1536,8 +1541,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.11206097854822998"/>
-                      <c:h val="4.7831682330031315E-2"/>
+                      <c:w val="0.11206097854823"/>
+                      <c:h val="0.0478316823300313"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -1562,8 +1567,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.11206097854822998"/>
-                      <c:h val="4.7831682330031315E-2"/>
+                      <c:w val="0.11206097854823"/>
+                      <c:h val="0.0478316823300313"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -1588,8 +1593,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.11206097854822998"/>
-                      <c:h val="4.7831682330031315E-2"/>
+                      <c:w val="0.11206097854823"/>
+                      <c:h val="0.0478316823300313"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -1778,8 +1783,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2085835224"/>
-        <c:axId val="2085832280"/>
+        <c:axId val="-2080321456"/>
+        <c:axId val="-2033775248"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1950,11 +1955,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2085841736"/>
-        <c:axId val="2085829160"/>
+        <c:axId val="-2080136768"/>
+        <c:axId val="-2033845808"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2085841736"/>
+        <c:axId val="-2080136768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1994,7 +1999,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085829160"/>
+        <c:crossAx val="-2033845808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2005,7 +2010,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2085829160"/>
+        <c:axId val="-2033845808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2015,12 +2020,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2085841736"/>
+        <c:crossAx val="-2080136768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2085832280"/>
+        <c:axId val="-2033775248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2030,12 +2035,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2085835224"/>
+        <c:crossAx val="-2080321456"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2085835224"/>
+        <c:axId val="-2080321456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2045,7 +2050,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2085832280"/>
+        <c:crossAx val="-2033775248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2564,7 +2569,7 @@
       <selection activeCell="C20" sqref="C20:C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
@@ -2578,7 +2583,7 @@
     <col min="14" max="14" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24.75" customHeight="1">
+    <row r="1" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="15" t="s">
         <v>7</v>
@@ -2596,7 +2601,7 @@
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
     </row>
-    <row r="2" spans="1:14" ht="28.5" customHeight="1">
+    <row r="2" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9"/>
       <c r="B2" s="13" t="s">
         <v>1</v>
@@ -2614,59 +2619,59 @@
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
     </row>
-    <row r="7" spans="1:14" ht="19.5" customHeight="1">
+    <row r="7" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:14" ht="19.5" customHeight="1">
+    <row r="8" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:14" ht="19.5" customHeight="1">
+    <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="19.5" customHeight="1">
+    <row r="10" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:14" ht="19.5" customHeight="1">
+    <row r="11" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:14" ht="19.5" customHeight="1">
+    <row r="12" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="19.5" customHeight="1">
+    <row r="13" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F13" s="1"/>
       <c r="I13" s="2"/>
       <c r="K13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" ht="19.5" customHeight="1">
+    <row r="14" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F14" s="1"/>
       <c r="I14" s="2"/>
       <c r="K14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" ht="19.5" customHeight="1">
+    <row r="15" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F15" s="1"/>
       <c r="I15" s="2"/>
       <c r="K15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="19.5" customHeight="1">
+    <row r="16" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F16" s="1"/>
       <c r="I16" s="2"/>
       <c r="K16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="2:14" ht="19.5" customHeight="1" thickBot="1">
+    <row r="17" spans="2:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="I17" s="2"/>
       <c r="K17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="2:14" ht="24" customHeight="1" thickTop="1">
+    <row r="18" spans="2:14" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B18" s="10" t="s">
         <v>6</v>
       </c>
@@ -2677,7 +2682,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="2:14" ht="24" customHeight="1">
+    <row r="19" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="6" t="s">
         <v>2</v>
       </c>
@@ -2696,7 +2701,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="2:14" ht="19.5" customHeight="1">
+    <row r="20" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="14">
         <v>42247</v>
       </c>
@@ -2715,7 +2720,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="2:14" ht="19.5" customHeight="1">
+    <row r="21" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="14">
         <v>42254</v>
       </c>
@@ -2735,7 +2740,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="2:14" ht="19.5" customHeight="1">
+    <row r="22" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="14">
         <v>42261</v>
       </c>
@@ -2754,7 +2759,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="2:14" ht="19.5" customHeight="1">
+    <row r="23" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="14">
         <v>42268</v>
       </c>
@@ -2773,7 +2778,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="2:14" ht="19.5" customHeight="1">
+    <row r="24" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="14">
         <v>42275</v>
       </c>
@@ -2792,7 +2797,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="2:14" ht="19.5" customHeight="1">
+    <row r="25" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="14">
         <v>42282</v>
       </c>
@@ -2811,7 +2816,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="2:14" ht="19.5" customHeight="1">
+    <row r="26" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="14">
         <v>42289</v>
       </c>
@@ -2830,7 +2835,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="2:14" ht="19.5" customHeight="1">
+    <row r="27" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="14">
         <v>42296</v>
       </c>
@@ -2845,7 +2850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:14" ht="19.5" customHeight="1">
+    <row r="28" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="14">
         <v>42303</v>
       </c>
@@ -2860,7 +2865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:14" ht="19.5" customHeight="1">
+    <row r="29" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="14">
         <v>42310</v>
       </c>
@@ -2876,7 +2881,7 @@
       </c>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="2:14" ht="19.5" customHeight="1">
+    <row r="30" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="14">
         <v>42317</v>
       </c>
@@ -2891,7 +2896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:14" ht="19.5" customHeight="1">
+    <row r="31" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="14">
         <v>42324</v>
       </c>
@@ -2906,7 +2911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:14" ht="19.5" customHeight="1">
+    <row r="32" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="14">
         <v>42331</v>
       </c>
@@ -2921,7 +2926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="19.5" customHeight="1">
+    <row r="33" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="14">
         <v>42338</v>
       </c>
@@ -2936,7 +2941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="19.5" customHeight="1">
+    <row r="34" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="14">
         <v>42345</v>
       </c>
@@ -2951,7 +2956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="19.5" customHeight="1">
+    <row r="35" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="14">
         <v>42352</v>
       </c>
@@ -2973,11 +2978,6 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2988,11 +2988,11 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.5" style="60" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" style="61" customWidth="1"/>
@@ -3002,7 +3002,7 @@
     <col min="6" max="16384" width="8.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="17" customFormat="1">
+    <row r="1" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="52" t="s">
         <v>24</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="2" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="54">
         <v>42247</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="19" customFormat="1" ht="48">
+    <row r="3" spans="1:5" s="19" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A3" s="54">
         <v>42247</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="4" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="54">
         <v>42247</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="19" customFormat="1" ht="24">
+    <row r="5" spans="1:5" s="19" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="54">
         <v>42251</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="6" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="54">
         <v>42254</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="19" customFormat="1" ht="56" customHeight="1">
+    <row r="7" spans="1:5" s="19" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="54">
         <v>42260</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="19" customFormat="1" ht="72">
+    <row r="8" spans="1:5" s="19" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A8" s="54">
         <v>42261</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="9" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="54">
         <v>42265</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="10" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="54" t="s">
         <v>104</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="11" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="54" t="s">
         <v>104</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="12" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="54">
         <v>42268</v>
       </c>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="D12" s="45"/>
     </row>
-    <row r="13" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="13" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="54">
         <v>42272</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="14" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="54">
         <v>42274</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="15" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="54">
         <v>42275</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="16" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="54">
         <v>42279</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="17" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="54">
         <v>42279</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="18" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="54">
         <v>42282</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="19" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="54">
         <v>42283</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="20" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="54">
         <v>42286</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="21" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="54">
         <v>42289</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="22" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="54">
         <v>42293</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="23" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="56">
         <v>42293</v>
       </c>
@@ -3326,7 +3326,7 @@
       </c>
       <c r="E23" s="51"/>
     </row>
-    <row r="24" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="24" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="54">
         <v>42296</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="25" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="54">
         <v>42300</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="26" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="54">
         <v>42302</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="27" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="54">
         <v>42305</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="28" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="54">
         <v>42307</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+    <row r="29" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="54">
         <v>42310</v>
       </c>
@@ -3406,9 +3406,11 @@
       <c r="C29" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="45"/>
-    </row>
-    <row r="30" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="D29" s="45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="54">
         <v>42317</v>
       </c>
@@ -3418,9 +3420,11 @@
       <c r="C30" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="45"/>
-    </row>
-    <row r="31" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1">
+      <c r="D30" s="45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="54">
         <v>42324</v>
       </c>
@@ -3430,9 +3434,11 @@
       <c r="C31" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="45"/>
-    </row>
-    <row r="32" spans="1:5" s="19" customFormat="1" ht="30" customHeight="1">
+      <c r="D31" s="45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="54">
         <v>42331</v>
       </c>
@@ -3442,9 +3448,11 @@
       <c r="C32" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="45"/>
-    </row>
-    <row r="33" spans="1:4" s="19" customFormat="1" ht="30" customHeight="1">
+      <c r="D32" s="45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="54">
         <v>42338</v>
       </c>
@@ -3454,9 +3462,11 @@
       <c r="C33" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="45"/>
-    </row>
-    <row r="34" spans="1:4" s="19" customFormat="1" ht="30" customHeight="1">
+      <c r="D33" s="45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="54">
         <v>42345</v>
       </c>
@@ -3466,9 +3476,11 @@
       <c r="C34" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="45"/>
-    </row>
-    <row r="35" spans="1:4" s="19" customFormat="1" ht="30" customHeight="1">
+      <c r="D34" s="45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="54">
         <v>42345</v>
       </c>
@@ -3482,7 +3494,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="19" customFormat="1" ht="30" customHeight="1">
+    <row r="36" spans="1:4" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="54">
         <v>42352</v>
       </c>
@@ -3496,92 +3508,92 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="37" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="58"/>
       <c r="B37" s="59"/>
       <c r="D37" s="47"/>
     </row>
-    <row r="38" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="38" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="58"/>
       <c r="B38" s="59"/>
       <c r="D38" s="47"/>
     </row>
-    <row r="39" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="39" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="58"/>
       <c r="B39" s="59"/>
       <c r="D39" s="47"/>
     </row>
-    <row r="40" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="40" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="58"/>
       <c r="B40" s="59"/>
       <c r="D40" s="47"/>
     </row>
-    <row r="41" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="41" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="58"/>
       <c r="B41" s="59"/>
       <c r="D41" s="47"/>
     </row>
-    <row r="42" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="42" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="58"/>
       <c r="B42" s="59"/>
       <c r="D42" s="47"/>
     </row>
-    <row r="43" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="43" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="58"/>
       <c r="B43" s="59"/>
       <c r="D43" s="47"/>
     </row>
-    <row r="44" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="44" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="58"/>
       <c r="B44" s="59"/>
       <c r="D44" s="47"/>
     </row>
-    <row r="45" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="45" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="58"/>
       <c r="B45" s="59"/>
       <c r="D45" s="47"/>
     </row>
-    <row r="46" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="46" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="58"/>
       <c r="B46" s="59"/>
       <c r="D46" s="47"/>
     </row>
-    <row r="47" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="47" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="58"/>
       <c r="B47" s="59"/>
       <c r="D47" s="47"/>
     </row>
-    <row r="48" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="48" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="58"/>
       <c r="B48" s="59"/>
       <c r="D48" s="47"/>
     </row>
-    <row r="49" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="49" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="58"/>
       <c r="B49" s="59"/>
       <c r="D49" s="47"/>
     </row>
-    <row r="50" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="50" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="58"/>
       <c r="B50" s="59"/>
       <c r="D50" s="47"/>
     </row>
-    <row r="51" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="51" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="58"/>
       <c r="B51" s="59"/>
       <c r="D51" s="47"/>
     </row>
-    <row r="52" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="52" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="58"/>
       <c r="B52" s="59"/>
       <c r="D52" s="47"/>
     </row>
-    <row r="53" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="53" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="58"/>
       <c r="B53" s="59"/>
       <c r="D53" s="47"/>
     </row>
-    <row r="54" spans="1:4" s="20" customFormat="1" ht="12">
+    <row r="54" spans="1:4" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="58"/>
       <c r="B54" s="59"/>
       <c r="D54" s="47"/>
@@ -3590,11 +3602,6 @@
   <printOptions gridLines="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="63" fitToHeight="0" orientation="landscape"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3606,7 +3613,7 @@
       <selection sqref="A1:D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="39.83203125" customWidth="1"/>
@@ -3614,7 +3621,7 @@
     <col min="4" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13">
+    <row r="1" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="21" t="s">
         <v>44</v>
       </c>
@@ -3628,7 +3635,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13">
+    <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="23" t="s">
         <v>48</v>
       </c>
@@ -3640,7 +3647,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13">
+    <row r="3" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="23"/>
       <c r="B3" s="24" t="s">
         <v>51</v>
@@ -3648,7 +3655,7 @@
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
     </row>
-    <row r="4" spans="1:4" ht="13">
+    <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="25" t="s">
         <v>52</v>
       </c>
@@ -3658,7 +3665,7 @@
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
     </row>
-    <row r="5" spans="1:4" ht="13">
+    <row r="5" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="23" t="s">
         <v>54</v>
       </c>
@@ -3672,13 +3679,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="13">
+    <row r="6" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="23"/>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
     </row>
-    <row r="7" spans="1:4" ht="13">
+    <row r="7" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="28" t="s">
         <v>57</v>
       </c>
@@ -3690,7 +3697,7 @@
       </c>
       <c r="D7" s="29"/>
     </row>
-    <row r="8" spans="1:4" ht="13">
+    <row r="8" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="23"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
@@ -3698,7 +3705,7 @@
       </c>
       <c r="D8" s="24"/>
     </row>
-    <row r="9" spans="1:4" ht="13">
+    <row r="9" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="30"/>
       <c r="B9" s="31"/>
       <c r="C9" s="32" t="s">
@@ -3706,7 +3713,7 @@
       </c>
       <c r="D9" s="31"/>
     </row>
-    <row r="10" spans="1:4" ht="15">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>62</v>
       </c>
@@ -3720,7 +3727,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13">
+    <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="23"/>
       <c r="B11" s="34"/>
       <c r="C11" s="24" t="s">
@@ -3728,7 +3735,7 @@
       </c>
       <c r="D11" s="24"/>
     </row>
-    <row r="12" spans="1:4" ht="13">
+    <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="23"/>
       <c r="B12" s="24"/>
       <c r="C12" s="27" t="s">
@@ -3736,7 +3743,7 @@
       </c>
       <c r="D12" s="24"/>
     </row>
-    <row r="13" spans="1:4" ht="13">
+    <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="28" t="s">
         <v>65</v>
       </c>
@@ -3750,7 +3757,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="13">
+    <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="30"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31" t="s">
@@ -3758,7 +3765,7 @@
       </c>
       <c r="D14" s="31"/>
     </row>
-    <row r="15" spans="1:4" ht="13">
+    <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="23" t="s">
         <v>66</v>
       </c>
@@ -3770,7 +3777,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="13">
+    <row r="16" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="23"/>
       <c r="B16" s="24"/>
       <c r="C16" s="31" t="s">
@@ -3780,7 +3787,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="13">
+    <row r="17" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="28" t="s">
         <v>69</v>
       </c>
@@ -3794,7 +3801,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="13">
+    <row r="18" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="30"/>
       <c r="B18" s="31" t="s">
         <v>92</v>
@@ -3804,7 +3811,7 @@
       </c>
       <c r="D18" s="31"/>
     </row>
-    <row r="19" spans="1:4" ht="13">
+    <row r="19" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="23" t="s">
         <v>71</v>
       </c>
@@ -3814,7 +3821,7 @@
       </c>
       <c r="D19" s="24"/>
     </row>
-    <row r="20" spans="1:4" ht="13">
+    <row r="20" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="23"/>
       <c r="B20" s="24"/>
       <c r="C20" s="24" t="s">
@@ -3822,7 +3829,7 @@
       </c>
       <c r="D20" s="24"/>
     </row>
-    <row r="21" spans="1:4" ht="13">
+    <row r="21" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="28" t="s">
         <v>72</v>
       </c>
@@ -3834,7 +3841,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="13">
+    <row r="22" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="30"/>
       <c r="B22" s="31"/>
       <c r="C22" s="32" t="s">
@@ -3844,7 +3851,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="13">
+    <row r="23" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="23" t="s">
         <v>75</v>
       </c>
@@ -3856,13 +3863,13 @@
       </c>
       <c r="D23" s="24"/>
     </row>
-    <row r="24" spans="1:4" ht="13">
+    <row r="24" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="23"/>
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
     </row>
-    <row r="25" spans="1:4" ht="13">
+    <row r="25" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="35" t="s">
         <v>77</v>
       </c>
@@ -3876,7 +3883,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="13">
+    <row r="26" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="37"/>
       <c r="B26" s="38"/>
       <c r="C26" s="24" t="s">
@@ -3884,7 +3891,7 @@
       </c>
       <c r="D26" s="31"/>
     </row>
-    <row r="27" spans="1:4" ht="13">
+    <row r="27" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="35" t="s">
         <v>78</v>
       </c>
@@ -3896,7 +3903,7 @@
       </c>
       <c r="D27" s="24"/>
     </row>
-    <row r="28" spans="1:4" ht="13">
+    <row r="28" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="30"/>
       <c r="B28" s="31"/>
       <c r="C28" s="31" t="s">
@@ -3904,7 +3911,7 @@
       </c>
       <c r="D28" s="24"/>
     </row>
-    <row r="29" spans="1:4" ht="13">
+    <row r="29" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="28" t="s">
         <v>80</v>
       </c>
@@ -3916,7 +3923,7 @@
       </c>
       <c r="D29" s="29"/>
     </row>
-    <row r="30" spans="1:4" ht="13">
+    <row r="30" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="30"/>
       <c r="B30" s="31" t="s">
         <v>90</v>
@@ -3926,7 +3933,7 @@
       </c>
       <c r="D30" s="31"/>
     </row>
-    <row r="31" spans="1:4" ht="13">
+    <row r="31" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="23" t="s">
         <v>81</v>
       </c>
@@ -3938,7 +3945,7 @@
       </c>
       <c r="D31" s="24"/>
     </row>
-    <row r="32" spans="1:4" ht="13">
+    <row r="32" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="23"/>
       <c r="B32" s="24" t="s">
         <v>93</v>
@@ -3948,7 +3955,7 @@
       </c>
       <c r="D32" s="24"/>
     </row>
-    <row r="33" spans="1:4" ht="13">
+    <row r="33" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="30"/>
       <c r="B33" s="31"/>
       <c r="C33" s="31" t="s">
@@ -3956,7 +3963,7 @@
       </c>
       <c r="D33" s="24"/>
     </row>
-    <row r="34" spans="1:4" ht="13">
+    <row r="34" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="28" t="s">
         <v>84</v>
       </c>
@@ -3968,7 +3975,7 @@
       </c>
       <c r="D34" s="29"/>
     </row>
-    <row r="35" spans="1:4" ht="13">
+    <row r="35" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="30"/>
       <c r="B35" s="31"/>
       <c r="C35" s="31" t="s">
@@ -3979,11 +3986,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3994,11 +3996,11 @@
   </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="B1" zoomScale="167" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="39"/>
     <col min="2" max="2" width="22.33203125" style="39" customWidth="1"/>
@@ -4007,12 +4009,12 @@
     <col min="5" max="16384" width="8.83203125" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="39" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="42" t="s">
         <v>24</v>
       </c>
@@ -4020,7 +4022,7 @@
         <v>42252</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="40" t="s">
         <v>95</v>
       </c>
@@ -4034,7 +4036,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
+    <row r="4" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="43" t="s">
         <v>98</v>
       </c>
@@ -4048,7 +4050,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
+    <row r="5" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="43" t="s">
         <v>101</v>
       </c>
@@ -4062,7 +4064,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
+    <row r="6" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="43" t="s">
         <v>99</v>
       </c>
@@ -4070,28 +4072,28 @@
       <c r="C6" s="44"/>
       <c r="D6" s="44"/>
     </row>
-    <row r="7" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
+    <row r="7" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="43"/>
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
     </row>
-    <row r="8" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
+    <row r="8" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="43"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
     </row>
-    <row r="9" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1">
+    <row r="9" spans="1:4" s="41" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="43"/>
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
       <c r="D9" s="44"/>
     </row>
-    <row r="10" spans="1:4" s="41" customFormat="1"/>
-    <row r="11" spans="1:4" s="41" customFormat="1"/>
-    <row r="12" spans="1:4" s="41" customFormat="1"/>
-    <row r="13" spans="1:4" s="41" customFormat="1"/>
+    <row r="10" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <conditionalFormatting sqref="A4:A8">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -4106,11 +4108,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="83" orientation="landscape"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added another responsible person
</commit_message>
<xml_diff>
--- a/HW 1/Project Plan.xlsx
+++ b/HW 1/Project Plan.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="153">
   <si>
     <t>Project Start</t>
   </si>
@@ -2988,8 +2988,8 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3169,7 +3169,9 @@
       <c r="C12" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="45"/>
+      <c r="D12" s="45" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:5" s="19" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="54">

</xml_diff>